<commit_message>
customized files from tufts, downloaded 1/23
</commit_message>
<xml_diff>
--- a/InputData/elec/BTaDLP/BAU Trans and Distr Loss Perc.xlsx
+++ b/InputData/elec/BTaDLP/BAU Trans and Distr Loss Perc.xlsx
@@ -264,11 +264,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="797790999"/>
-        <c:axId val="384305320"/>
+        <c:axId val="738518057"/>
+        <c:axId val="1091508992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="797790999"/>
+        <c:axId val="738518057"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -320,10 +320,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="384305320"/>
+        <c:crossAx val="1091508992"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="384305320"/>
+        <c:axId val="1091508992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -398,7 +398,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="797790999"/>
+        <c:crossAx val="738518057"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>

</xml_diff>

<commit_message>
customized files from tufts, downloaded 1/25
</commit_message>
<xml_diff>
--- a/InputData/elec/BTaDLP/BAU Trans and Distr Loss Perc.xlsx
+++ b/InputData/elec/BTaDLP/BAU Trans and Distr Loss Perc.xlsx
@@ -264,11 +264,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="738518057"/>
-        <c:axId val="1091508992"/>
+        <c:axId val="347946214"/>
+        <c:axId val="1685555507"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="738518057"/>
+        <c:axId val="347946214"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -320,10 +320,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1091508992"/>
+        <c:crossAx val="1685555507"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1091508992"/>
+        <c:axId val="1685555507"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -398,7 +398,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="738518057"/>
+        <c:crossAx val="347946214"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>

</xml_diff>